<commit_message>
rewriiten for new grating
</commit_message>
<xml_diff>
--- a/Gratingmeasurements.xlsx
+++ b/Gratingmeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stuart Smyth\Documents\GitHub\gMOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{965329EE-C8FD-47C0-A12E-42A6EFD3DCE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11650DE0-FBE5-46C8-AE0A-64252560428C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{ED76D3F0-AE17-4DCB-B648-01C91423C949}"/>
   </bookViews>
@@ -25,48 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Grating 1</t>
-  </si>
-  <si>
-    <t>Grating 4</t>
-  </si>
-  <si>
-    <t>Grating 3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>I(uW)</t>
   </si>
   <si>
-    <t>Io(uW)</t>
-  </si>
-  <si>
     <t>F1 I1(uW)</t>
   </si>
   <si>
     <t>F1 Iv(uW)</t>
   </si>
   <si>
-    <t>F1 Ih (uW)</t>
-  </si>
-  <si>
     <t>F2 I1(uW)</t>
   </si>
   <si>
     <t>F2 Iv(uW)</t>
   </si>
   <si>
-    <t>F2 Ih(uW)</t>
-  </si>
-  <si>
     <t>F3 I1(uW)</t>
   </si>
   <si>
     <t>F3 Iv(uW)</t>
   </si>
   <si>
-    <t>F3 Ih(uW)</t>
+    <t xml:space="preserve">Grating 5 </t>
+  </si>
+  <si>
+    <t>F1 Io(uW)</t>
+  </si>
+  <si>
+    <t>F2 Io (uW)</t>
+  </si>
+  <si>
+    <t>F3 Io(uW)</t>
   </si>
 </sst>
 </file>
@@ -418,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C06C11-68C6-40C0-AE5A-5B285E0C7AE3}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,153 +429,71 @@
     <col min="10" max="10" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>861.4</v>
+        <v>974.7</v>
       </c>
       <c r="C2">
-        <v>597</v>
+        <v>70.7</v>
       </c>
       <c r="D2">
-        <v>480</v>
+        <v>369.8</v>
       </c>
       <c r="E2">
-        <v>128.1</v>
+        <v>337.2</v>
       </c>
       <c r="F2">
-        <v>300.60000000000002</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="G2">
-        <v>500</v>
+        <v>346</v>
       </c>
       <c r="H2">
-        <v>129</v>
+        <v>321</v>
       </c>
       <c r="I2">
-        <v>319</v>
+        <v>71.2</v>
       </c>
       <c r="J2">
-        <v>505.6</v>
+        <v>368</v>
       </c>
       <c r="K2">
-        <v>138</v>
-      </c>
-      <c r="L2">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1131</v>
-      </c>
-      <c r="C3">
-        <v>985.5</v>
-      </c>
-      <c r="D3">
-        <v>427</v>
-      </c>
-      <c r="E3">
-        <v>361</v>
-      </c>
-      <c r="F3">
-        <v>62.2</v>
-      </c>
-      <c r="G3">
-        <v>441</v>
-      </c>
-      <c r="H3">
-        <v>374</v>
-      </c>
-      <c r="I3">
-        <v>54.5</v>
-      </c>
-      <c r="J3">
-        <v>410</v>
-      </c>
-      <c r="K3">
-        <v>368</v>
-      </c>
-      <c r="L3">
-        <v>43.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1131</v>
-      </c>
-      <c r="C4">
-        <v>1001</v>
-      </c>
-      <c r="D4">
-        <v>435.6</v>
-      </c>
-      <c r="E4">
-        <v>345</v>
-      </c>
-      <c r="F4">
-        <v>44</v>
-      </c>
-      <c r="G4">
-        <v>399</v>
-      </c>
-      <c r="H4">
-        <v>341</v>
-      </c>
-      <c r="I4">
-        <v>43.4</v>
-      </c>
-      <c r="J4">
-        <v>379</v>
-      </c>
-      <c r="K4">
-        <v>332</v>
-      </c>
-      <c r="L4">
-        <v>49.6</v>
+        <v>320.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after retaking of data
</commit_message>
<xml_diff>
--- a/Gratingmeasurements.xlsx
+++ b/Gratingmeasurements.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stuart Smyth\Documents\GitHub\gMOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11650DE0-FBE5-46C8-AE0A-64252560428C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94D0FB2-6488-462A-A0F6-90142D690C25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{ED76D3F0-AE17-4DCB-B648-01C91423C949}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>I(uW)</t>
   </si>
@@ -58,6 +63,12 @@
   </si>
   <si>
     <t>F3 Io(uW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grating 1 </t>
+  </si>
+  <si>
+    <t>Grating 3</t>
   </si>
 </sst>
 </file>
@@ -409,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C06C11-68C6-40C0-AE5A-5B285E0C7AE3}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,6 +507,95 @@
         <v>320.7</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>998.1+7.63</f>
+        <v>1005.73</v>
+      </c>
+      <c r="C3">
+        <f>56.8+17.8</f>
+        <v>74.599999999999994</v>
+      </c>
+      <c r="D3">
+        <f>372+11</f>
+        <v>383</v>
+      </c>
+      <c r="E3">
+        <f>306+36.3</f>
+        <v>342.3</v>
+      </c>
+      <c r="F3">
+        <f>50.2+17.8</f>
+        <v>68</v>
+      </c>
+      <c r="G3">
+        <f>350+11</f>
+        <v>361</v>
+      </c>
+      <c r="H3">
+        <f>305.6+36.3</f>
+        <v>341.90000000000003</v>
+      </c>
+      <c r="I3">
+        <f xml:space="preserve"> 53.53+17.8</f>
+        <v>71.33</v>
+      </c>
+      <c r="J3">
+        <f>357.4+11</f>
+        <v>368.4</v>
+      </c>
+      <c r="K3">
+        <f>323.2+36.3</f>
+        <v>359.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1005.73</v>
+      </c>
+      <c r="C4">
+        <f>99.8+17.8</f>
+        <v>117.6</v>
+      </c>
+      <c r="D4">
+        <f>345+11</f>
+        <v>356</v>
+      </c>
+      <c r="E4">
+        <f>295.5+36.3</f>
+        <v>331.8</v>
+      </c>
+      <c r="F4">
+        <f xml:space="preserve"> 62.96+17.8</f>
+        <v>80.760000000000005</v>
+      </c>
+      <c r="G4">
+        <f>376.8+11</f>
+        <v>387.8</v>
+      </c>
+      <c r="H4">
+        <f>326.3+36.3</f>
+        <v>362.6</v>
+      </c>
+      <c r="I4">
+        <f>66.93+17.8</f>
+        <v>84.73</v>
+      </c>
+      <c r="J4">
+        <f>353.7+11</f>
+        <v>364.7</v>
+      </c>
+      <c r="K4">
+        <f xml:space="preserve"> 303.8+36.3</f>
+        <v>340.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>